<commit_message>
:sparkles: Projeto funcionando em partes
Falta apenas deixar as partes trabalhando juntas, colocar anotações e nomes sugestivos, e por fim, melhorar fluxo desenvolvido
</commit_message>
<xml_diff>
--- a/ProjetoSmarthis/Data/Input/InputDataFilter.xlsx
+++ b/ProjetoSmarthis/Data/Input/InputDataFilter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Documents\GitHub\UiPath\ProjetoSmarthis\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26074268-870B-4C2D-8D43-B25771EC2D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D703AB9F-AE8B-4301-A968-90B5EE5D416B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5772" yWindow="2328" windowWidth="16368" windowHeight="8628" xr2:uid="{5BD2685B-9114-40EC-A527-CB51483A8D51}"/>
+    <workbookView xWindow="5115" yWindow="855" windowWidth="15375" windowHeight="7875" xr2:uid="{FE399519-DCEB-48EE-974A-BAEB9C118F02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -420,14 +420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28806790-12C8-41DE-82F5-8F5B6D088564}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84E5371-8255-433E-8A0F-3CEEDCA7514E}">
   <dimension ref="A1:C151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -449,7 +449,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -460,7 +460,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -471,7 +471,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -482,7 +482,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -493,7 +493,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -504,7 +504,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -515,7 +515,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -526,7 +526,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -537,7 +537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -548,7 +548,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -559,7 +559,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -570,7 +570,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -592,7 +592,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -603,7 +603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -614,7 +614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -625,7 +625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -636,7 +636,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -647,7 +647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -658,7 +658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -669,7 +669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -680,7 +680,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -691,7 +691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -702,7 +702,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -713,7 +713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -724,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -735,7 +735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -746,7 +746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -757,7 +757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -768,7 +768,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -790,7 +790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -801,7 +801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -812,7 +812,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -823,7 +823,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -834,7 +834,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -845,7 +845,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -856,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -867,7 +867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -878,7 +878,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -889,7 +889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -900,7 +900,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -911,7 +911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -922,7 +922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -933,7 +933,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -944,7 +944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -955,7 +955,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -966,7 +966,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -977,7 +977,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -999,7 +999,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>7</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>7</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>3</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>7</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>7</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>6</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>7</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -2094,12 +2094,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8017C9CC-21B0-4A7D-9E4A-577B4A5EE8A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044C8BDC-868D-4F98-B478-AD30BBC06C66}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>